<commit_message>
Re-ran platform tests post beta release builds and documented
</commit_message>
<xml_diff>
--- a/windows/src/test/manual-tests/platform-rules/platform-results.xlsx
+++ b/windows/src/test/manual-tests/platform-rules/platform-results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="116">
   <si>
     <t>touch</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Windows 10.0.16299.371</t>
   </si>
   <si>
-    <t>10.0.299</t>
-  </si>
-  <si>
     <t>iOS</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>Linux Ubuntu 16.04 LTS</t>
   </si>
   <si>
-    <t>10.0.153</t>
-  </si>
-  <si>
     <t>10.0.47</t>
   </si>
   <si>
@@ -296,9 +290,6 @@
     <t>hardware windows desktop web ie !touch undefined windows</t>
   </si>
   <si>
-    <t>hardware windows desktop web undefined !touch undefined windows</t>
-  </si>
-  <si>
     <t>hardware windows desktop web opera !touch undefined windows</t>
   </si>
   <si>
@@ -332,14 +323,62 @@
     <t>hardware ios tablet web safari !touch undefined ios</t>
   </si>
   <si>
-    <t>touch android phone native undefined !hardware platform-x android</t>
+    <t>10.0.93</t>
+  </si>
+  <si>
+    <t>hardware windows desktop web edge !touch undefined windows</t>
+  </si>
+  <si>
+    <t>10.0.92</t>
+  </si>
+  <si>
+    <t>touch ios phone web safari !hardware undefined ios</t>
+  </si>
+  <si>
+    <t>touch ios phone native undefined !hardware undefined ios</t>
+  </si>
+  <si>
+    <t>touch ios tablet native undefined !hardware undefined ios</t>
+  </si>
+  <si>
+    <t>10.0.155</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>N/A N/A N/A N/A N/A N/A N/A N/A</t>
+  </si>
+  <si>
+    <t>touch android tablet web chrome !hardware undefined android</t>
+  </si>
+  <si>
+    <t>hardware android tablet web chrome !touch undefined android</t>
+  </si>
+  <si>
+    <t>touch android phone native undefined !hardware undefined android</t>
+  </si>
+  <si>
+    <t>hardware android phone native undefined !touch undefined android</t>
+  </si>
+  <si>
+    <t>touch android tablet native undefined !hardware undefined android</t>
+  </si>
+  <si>
+    <t>hardware android tablet native undefined !touch undefined android</t>
+  </si>
+  <si>
+    <t>10.0.399</t>
+  </si>
+  <si>
+    <t>*not responding to hardware keyboard; separate issue?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +397,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -439,7 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -504,12 +549,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -553,459 +592,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1349,13 +961,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W79"/>
+  <dimension ref="A1:X79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomRight" activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,74 +998,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="40"/>
-      <c r="H1" s="26" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="44"/>
+      <c r="J1" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="44"/>
+      <c r="L1" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="26" t="s">
+      <c r="M1" s="44"/>
+      <c r="N1" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="26" t="s">
+      <c r="O1" s="44"/>
+      <c r="P1" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="26" t="s">
+      <c r="Q1" s="44"/>
+      <c r="R1" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="44"/>
+      <c r="T1" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="26" t="s">
+      <c r="U1" s="44"/>
+      <c r="V1" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="44"/>
+    </row>
+    <row r="2" spans="1:23" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="38"/>
+      <c r="H2" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="44"/>
+      <c r="J2" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="K2" s="44"/>
+      <c r="L2" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="44"/>
+      <c r="N2" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="O2" s="44"/>
+      <c r="P2" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" s="44"/>
+      <c r="T2" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="26" t="s">
+      <c r="U2" s="44"/>
+      <c r="V2" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="S1" s="27"/>
-      <c r="T1" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="U1" s="27"/>
-      <c r="V1" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="W1" s="27"/>
-    </row>
-    <row r="2" spans="1:23" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="G2" s="40"/>
-      <c r="H2" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="M2" s="27"/>
-      <c r="N2" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" s="27"/>
-      <c r="T2" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="U2" s="27"/>
-      <c r="V2" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="W2" s="27"/>
+      <c r="W2" s="44"/>
     </row>
     <row r="3" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -1474,114 +1086,114 @@
       <c r="F3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="40" t="s">
+      <c r="G3" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="31" customFormat="1" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" s="33" customFormat="1" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="35">
+      <c r="G4" s="39"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="33">
         <v>1</v>
       </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="35">
+      <c r="J4" s="34"/>
+      <c r="K4" s="33">
         <v>2</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="35">
+      <c r="L4" s="34"/>
+      <c r="M4" s="33">
         <v>3</v>
       </c>
-      <c r="N4" s="36"/>
-      <c r="O4" s="35">
+      <c r="N4" s="34"/>
+      <c r="O4" s="33">
         <v>4</v>
       </c>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="35">
+      <c r="P4" s="34"/>
+      <c r="Q4" s="33">
         <v>5</v>
       </c>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37">
+      <c r="R4" s="35"/>
+      <c r="S4" s="35">
         <v>6</v>
       </c>
-      <c r="T4" s="34"/>
-      <c r="U4" s="35">
+      <c r="T4" s="32"/>
+      <c r="U4" s="33">
         <v>7</v>
       </c>
       <c r="V4" s="11"/>
-      <c r="W4" s="38">
+      <c r="W4" s="36">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="42"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="29"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="29"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="27"/>
       <c r="R5" s="25"/>
       <c r="S5" s="25"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="32"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="30"/>
       <c r="V5" s="23"/>
-      <c r="W5" s="28"/>
+      <c r="W5" s="26"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1591,8 +1203,8 @@
       <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
-        <v>80</v>
+      <c r="D6" s="42" t="s">
+        <v>78</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>31</v>
@@ -1600,8 +1212,8 @@
       <c r="F6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="44" t="s">
-        <v>85</v>
+      <c r="G6" s="42" t="s">
+        <v>83</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>1</v>
@@ -1632,21 +1244,21 @@
         <v>native</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q6" s="14" t="str">
         <f>TRIM(MID(SUBSTITUTE($G6," ",REPT(" ",LEN($G6))), (Q$4-1)*LEN($G6)+1, LEN($G6)))</f>
         <v>undefined</v>
       </c>
       <c r="R6" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S6" s="14" t="str">
         <f>TRIM(MID(SUBSTITUTE($G6," ",REPT(" ",LEN($G6))), (S$4-1)*LEN($G6)+1, LEN($G6)))</f>
         <v>!touch</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U6" s="14" t="str">
         <f>TRIM(MID(SUBSTITUTE($G6," ",REPT(" ",LEN($G6))), (U$4-1)*LEN($G6)+1, LEN($G6)))</f>
@@ -1667,8 +1279,8 @@
       <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
-        <v>80</v>
+      <c r="D7" s="42" t="s">
+        <v>78</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
@@ -1676,8 +1288,8 @@
       <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="44" t="s">
-        <v>85</v>
+      <c r="G7" s="42" t="s">
+        <v>83</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>1</v>
@@ -1708,21 +1320,21 @@
         <v>native</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q7" s="14" t="str">
         <f t="shared" ref="Q7:Q56" si="4">TRIM(MID(SUBSTITUTE($G7," ",REPT(" ",LEN($G7))), (Q$4-1)*LEN($G7)+1, LEN($G7)))</f>
         <v>undefined</v>
       </c>
       <c r="R7" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S7" s="14" t="str">
         <f t="shared" ref="S7:S56" si="5">TRIM(MID(SUBSTITUTE($G7," ",REPT(" ",LEN($G7))), (S$4-1)*LEN($G7)+1, LEN($G7)))</f>
         <v>!touch</v>
       </c>
       <c r="T7" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U7" s="14" t="str">
         <f t="shared" ref="U7:U56" si="6">TRIM(MID(SUBSTITUTE($G7," ",REPT(" ",LEN($G7))), (U$4-1)*LEN($G7)+1, LEN($G7)))</f>
@@ -1743,8 +1355,8 @@
       <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
-        <v>47</v>
+      <c r="D8" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
@@ -1752,8 +1364,8 @@
       <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="44" t="s">
-        <v>88</v>
+      <c r="G8" s="42" t="s">
+        <v>86</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>1</v>
@@ -1791,14 +1403,14 @@
         <v>chrome</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S8" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T8" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U8" s="14" t="str">
         <f t="shared" si="6"/>
@@ -1819,8 +1431,8 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
-        <v>47</v>
+      <c r="D9" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E9" t="s">
         <v>45</v>
@@ -1828,8 +1440,8 @@
       <c r="F9" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="44" t="s">
-        <v>89</v>
+      <c r="G9" s="42" t="s">
+        <v>87</v>
       </c>
       <c r="H9" s="18" t="s">
         <v>1</v>
@@ -1867,14 +1479,14 @@
         <v>ie</v>
       </c>
       <c r="R9" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S9" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T9" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U9" s="14" t="str">
         <f t="shared" si="6"/>
@@ -1895,8 +1507,8 @@
       <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" t="s">
-        <v>47</v>
+      <c r="D10" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
@@ -1904,8 +1516,8 @@
       <c r="F10" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="44" t="s">
-        <v>90</v>
+      <c r="G10" s="42" t="s">
+        <v>100</v>
       </c>
       <c r="H10" s="18" t="s">
         <v>1</v>
@@ -1936,21 +1548,21 @@
         <v>web</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q10" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>undefined</v>
+        <v>edge</v>
       </c>
       <c r="R10" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S10" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T10" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U10" s="14" t="str">
         <f t="shared" si="6"/>
@@ -1971,8 +1583,8 @@
       <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" t="s">
-        <v>47</v>
+      <c r="D11" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E11" t="s">
         <v>42</v>
@@ -1980,8 +1592,8 @@
       <c r="F11" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="44" t="s">
-        <v>91</v>
+      <c r="G11" s="42" t="s">
+        <v>88</v>
       </c>
       <c r="H11" s="18" t="s">
         <v>1</v>
@@ -2019,14 +1631,14 @@
         <v>opera</v>
       </c>
       <c r="R11" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S11" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T11" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U11" s="14" t="str">
         <f t="shared" si="6"/>
@@ -2047,8 +1659,8 @@
       <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
-        <v>47</v>
+      <c r="D12" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
@@ -2056,8 +1668,8 @@
       <c r="F12" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="44" t="s">
-        <v>92</v>
+      <c r="G12" s="42" t="s">
+        <v>89</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>1</v>
@@ -2095,14 +1707,14 @@
         <v>firefox</v>
       </c>
       <c r="R12" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S12" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T12" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U12" s="14" t="str">
         <f t="shared" si="6"/>
@@ -2117,7 +1729,7 @@
       </c>
     </row>
     <row r="13" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="43"/>
+      <c r="G13" s="41"/>
       <c r="H13" s="21"/>
       <c r="I13" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2161,22 +1773,22 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
         <v>54</v>
-      </c>
-      <c r="E14" t="s">
-        <v>56</v>
       </c>
       <c r="F14" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="44" t="s">
-        <v>87</v>
+      <c r="G14" s="42" t="s">
+        <v>85</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>1</v>
@@ -2207,21 +1819,21 @@
         <v>native</v>
       </c>
       <c r="P14" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q14" s="14" t="str">
         <f t="shared" si="4"/>
         <v>undefined</v>
       </c>
       <c r="R14" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S14" s="14" t="str">
         <f t="shared" si="5"/>
         <v>undefined</v>
       </c>
       <c r="T14" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U14" s="14" t="str">
         <f t="shared" si="6"/>
@@ -2237,13 +1849,13 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" t="s">
-        <v>47</v>
+      <c r="D15" s="42" t="s">
+        <v>101</v>
       </c>
       <c r="E15" t="s">
         <v>21</v>
@@ -2251,8 +1863,8 @@
       <c r="F15" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="44" t="s">
-        <v>93</v>
+      <c r="G15" s="42" t="s">
+        <v>90</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>1</v>
@@ -2290,14 +1902,14 @@
         <v>chrome</v>
       </c>
       <c r="R15" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S15" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T15" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U15" s="14" t="str">
         <f t="shared" si="6"/>
@@ -2313,13 +1925,13 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
       </c>
-      <c r="D16" t="s">
-        <v>47</v>
+      <c r="D16" s="42" t="s">
+        <v>101</v>
       </c>
       <c r="E16" t="s">
         <v>44</v>
@@ -2327,8 +1939,8 @@
       <c r="F16" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="44" t="s">
-        <v>94</v>
+      <c r="G16" s="42" t="s">
+        <v>91</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>1</v>
@@ -2366,14 +1978,14 @@
         <v>safari</v>
       </c>
       <c r="R16" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S16" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T16" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U16" s="14" t="str">
         <f t="shared" si="6"/>
@@ -2387,15 +1999,15 @@
         <v>macosx</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="D17" t="s">
-        <v>47</v>
+      <c r="D17" s="42" t="s">
+        <v>101</v>
       </c>
       <c r="E17" t="s">
         <v>41</v>
@@ -2403,8 +2015,8 @@
       <c r="F17" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="44" t="s">
-        <v>95</v>
+      <c r="G17" s="42" t="s">
+        <v>92</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>1</v>
@@ -2442,14 +2054,14 @@
         <v>firefox</v>
       </c>
       <c r="R17" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S17" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T17" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U17" s="14" t="str">
         <f t="shared" si="6"/>
@@ -2463,8 +2075,8 @@
         <v>macosx</v>
       </c>
     </row>
-    <row r="18" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G18" s="43"/>
+    <row r="18" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="41"/>
       <c r="H18" s="21"/>
       <c r="I18" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2506,15 +2118,15 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
       </c>
-      <c r="D19" t="s">
-        <v>47</v>
+      <c r="D19" s="42" t="s">
+        <v>101</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
@@ -2522,8 +2134,8 @@
       <c r="F19" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="44" t="s">
-        <v>96</v>
+      <c r="G19" s="42" t="s">
+        <v>93</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>1</v>
@@ -2561,14 +2173,14 @@
         <v>chrome</v>
       </c>
       <c r="R19" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S19" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T19" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U19" s="14" t="str">
         <f t="shared" si="6"/>
@@ -2582,15 +2194,15 @@
         <v>linux</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="D20" t="s">
-        <v>47</v>
+      <c r="D20" s="42" t="s">
+        <v>101</v>
       </c>
       <c r="E20" t="s">
         <v>41</v>
@@ -2598,8 +2210,8 @@
       <c r="F20" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="44" t="s">
-        <v>97</v>
+      <c r="G20" s="42" t="s">
+        <v>94</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>1</v>
@@ -2637,14 +2249,14 @@
         <v>firefox</v>
       </c>
       <c r="R20" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S20" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T20" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U20" s="14" t="str">
         <f t="shared" si="6"/>
@@ -2658,8 +2270,8 @@
         <v>linux</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="43"/>
+    <row r="21" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="41"/>
       <c r="H21" s="21"/>
       <c r="I21" s="14" t="str">
         <f t="shared" si="0"/>
@@ -2701,9 +2313,9 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
@@ -2711,8 +2323,8 @@
       <c r="C22" t="s">
         <v>34</v>
       </c>
-      <c r="D22" t="s">
-        <v>47</v>
+      <c r="D22" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E22" t="s">
         <v>21</v>
@@ -2720,67 +2332,69 @@
       <c r="F22" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="44"/>
+      <c r="G22" s="42" t="s">
+        <v>96</v>
+      </c>
       <c r="H22" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I22" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K22" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>android</v>
       </c>
       <c r="L22" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M22" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>phone</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>11</v>
       </c>
       <c r="O22" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>web</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>13</v>
       </c>
       <c r="Q22" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>chrome</v>
       </c>
       <c r="R22" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S22" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T22" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U22" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V22" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W22" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+        <v>android</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -2788,8 +2402,8 @@
       <c r="C23" t="s">
         <v>34</v>
       </c>
-      <c r="D23" t="s">
-        <v>47</v>
+      <c r="D23" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E23" t="s">
         <v>21</v>
@@ -2797,67 +2411,72 @@
       <c r="F23" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="44"/>
+      <c r="G23" s="42" t="s">
+        <v>107</v>
+      </c>
       <c r="H23" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I23" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="J23" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K23" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M23" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="N23" s="6" t="s">
         <v>11</v>
       </c>
       <c r="O23" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="P23" s="6" t="s">
         <v>13</v>
       </c>
       <c r="Q23" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="R23" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S23" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="T23" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U23" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="V23" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W23" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+        <v>N/A</v>
+      </c>
+      <c r="X23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
         <v>26</v>
@@ -2865,14 +2484,17 @@
       <c r="C24" t="s">
         <v>35</v>
       </c>
+      <c r="D24" s="42" t="s">
+        <v>114</v>
+      </c>
       <c r="E24" t="s">
         <v>28</v>
       </c>
       <c r="F24" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="44" t="s">
-        <v>102</v>
+      <c r="G24" s="42" t="s">
+        <v>110</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>0</v>
@@ -2903,25 +2525,25 @@
         <v>native</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q24" s="14" t="str">
         <f t="shared" si="4"/>
         <v>undefined</v>
       </c>
       <c r="R24" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S24" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!hardware</v>
       </c>
       <c r="T24" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U24" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>platform-x</v>
+        <v>undefined</v>
       </c>
       <c r="V24" s="15" t="s">
         <v>3</v>
@@ -2931,9 +2553,9 @@
         <v>android</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
         <v>26</v>
@@ -2941,73 +2563,78 @@
       <c r="C25" t="s">
         <v>35</v>
       </c>
+      <c r="D25" s="42" t="s">
+        <v>114</v>
+      </c>
       <c r="E25" t="s">
         <v>28</v>
       </c>
       <c r="F25" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="44"/>
+      <c r="G25" s="42" t="s">
+        <v>111</v>
+      </c>
       <c r="H25" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I25" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>hardware</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K25" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>android</v>
       </c>
       <c r="L25" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M25" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>phone</v>
       </c>
       <c r="N25" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O25" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P25" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q25" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R25" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S25" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!touch</v>
       </c>
       <c r="T25" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U25" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V25" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W25" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+        <v>android</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -3015,73 +2642,78 @@
       <c r="C26" t="s">
         <v>35</v>
       </c>
+      <c r="D26" s="42" t="s">
+        <v>114</v>
+      </c>
       <c r="E26" t="s">
         <v>29</v>
       </c>
       <c r="F26" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="44"/>
+      <c r="G26" s="42" t="s">
+        <v>110</v>
+      </c>
       <c r="H26" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I26" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K26" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>android</v>
       </c>
       <c r="L26" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M26" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>phone</v>
       </c>
       <c r="N26" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O26" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q26" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R26" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S26" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T26" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U26" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V26" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W26" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+        <v>android</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -3089,73 +2721,78 @@
       <c r="C27" t="s">
         <v>35</v>
       </c>
+      <c r="D27" s="42" t="s">
+        <v>114</v>
+      </c>
       <c r="E27" t="s">
         <v>29</v>
       </c>
       <c r="F27" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="44"/>
+      <c r="G27" s="42" t="s">
+        <v>111</v>
+      </c>
       <c r="H27" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I27" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>hardware</v>
       </c>
       <c r="J27" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K27" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>android</v>
       </c>
       <c r="L27" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M27" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>phone</v>
       </c>
       <c r="N27" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O27" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q27" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R27" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S27" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!touch</v>
       </c>
       <c r="T27" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U27" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V27" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W27" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+        <v>android</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -3163,8 +2800,8 @@
       <c r="C28" t="s">
         <v>34</v>
       </c>
-      <c r="D28" t="s">
-        <v>47</v>
+      <c r="D28" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E28" t="s">
         <v>21</v>
@@ -3172,67 +2809,69 @@
       <c r="F28" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="44"/>
+      <c r="G28" s="42" t="s">
+        <v>108</v>
+      </c>
       <c r="H28" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I28" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J28" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K28" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>android</v>
       </c>
       <c r="L28" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M28" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>tablet</v>
       </c>
       <c r="N28" s="6" t="s">
         <v>11</v>
       </c>
       <c r="O28" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>web</v>
       </c>
       <c r="P28" s="6" t="s">
         <v>13</v>
       </c>
       <c r="Q28" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>chrome</v>
       </c>
       <c r="R28" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S28" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T28" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U28" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V28" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W28" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+        <v>android</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
         <v>40</v>
@@ -3240,8 +2879,8 @@
       <c r="C29" t="s">
         <v>34</v>
       </c>
-      <c r="D29" t="s">
-        <v>47</v>
+      <c r="D29" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E29" t="s">
         <v>21</v>
@@ -3249,67 +2888,69 @@
       <c r="F29" t="s">
         <v>27</v>
       </c>
-      <c r="G29" s="44"/>
+      <c r="G29" s="42" t="s">
+        <v>109</v>
+      </c>
       <c r="H29" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I29" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>hardware</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K29" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>android</v>
       </c>
       <c r="L29" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M29" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>tablet</v>
       </c>
       <c r="N29" s="6" t="s">
         <v>11</v>
       </c>
       <c r="O29" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>web</v>
       </c>
       <c r="P29" s="6" t="s">
         <v>13</v>
       </c>
       <c r="Q29" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>chrome</v>
       </c>
       <c r="R29" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S29" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!touch</v>
       </c>
       <c r="T29" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U29" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V29" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W29" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+        <v>android</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
         <v>40</v>
@@ -3317,73 +2958,78 @@
       <c r="C30" t="s">
         <v>35</v>
       </c>
+      <c r="D30" s="42" t="s">
+        <v>114</v>
+      </c>
       <c r="E30" t="s">
         <v>28</v>
       </c>
       <c r="F30" t="s">
         <v>36</v>
       </c>
-      <c r="G30" s="44"/>
+      <c r="G30" s="42" t="s">
+        <v>112</v>
+      </c>
       <c r="H30" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I30" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K30" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>android</v>
       </c>
       <c r="L30" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M30" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>tablet</v>
       </c>
       <c r="N30" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O30" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P30" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q30" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R30" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S30" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T30" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U30" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V30" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W30" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+        <v>android</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
         <v>40</v>
@@ -3391,73 +3037,78 @@
       <c r="C31" t="s">
         <v>35</v>
       </c>
+      <c r="D31" s="42" t="s">
+        <v>114</v>
+      </c>
       <c r="E31" t="s">
         <v>28</v>
       </c>
       <c r="F31" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="44"/>
+      <c r="G31" s="42" t="s">
+        <v>113</v>
+      </c>
       <c r="H31" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I31" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>hardware</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K31" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>android</v>
       </c>
       <c r="L31" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M31" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>tablet</v>
       </c>
       <c r="N31" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O31" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q31" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R31" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S31" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!touch</v>
       </c>
       <c r="T31" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U31" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V31" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W31" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+        <v>android</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
@@ -3465,73 +3116,78 @@
       <c r="C32" t="s">
         <v>35</v>
       </c>
+      <c r="D32" s="42" t="s">
+        <v>114</v>
+      </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="44"/>
+      <c r="G32" s="42" t="s">
+        <v>112</v>
+      </c>
       <c r="H32" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I32" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J32" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K32" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>android</v>
       </c>
       <c r="L32" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M32" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>tablet</v>
       </c>
       <c r="N32" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O32" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P32" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q32" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R32" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S32" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T32" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U32" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V32" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W32" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>android</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
@@ -3539,72 +3195,77 @@
       <c r="C33" t="s">
         <v>35</v>
       </c>
+      <c r="D33" s="42" t="s">
+        <v>114</v>
+      </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F33" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="44"/>
+      <c r="G33" s="42" t="s">
+        <v>113</v>
+      </c>
       <c r="H33" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I33" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>hardware</v>
       </c>
       <c r="J33" s="6" t="s">
         <v>3</v>
       </c>
       <c r="K33" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>android</v>
       </c>
       <c r="L33" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M33" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>tablet</v>
       </c>
       <c r="N33" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O33" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P33" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q33" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R33" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S33" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!touch</v>
       </c>
       <c r="T33" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U33" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V33" s="15" t="s">
         <v>3</v>
       </c>
       <c r="W33" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>android</v>
       </c>
     </row>
     <row r="34" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G34" s="43"/>
+      <c r="G34" s="41"/>
       <c r="H34" s="21"/>
       <c r="I34" s="14" t="str">
         <f t="shared" si="0"/>
@@ -3648,7 +3309,7 @@
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
         <v>26</v>
@@ -3656,8 +3317,8 @@
       <c r="C35" t="s">
         <v>34</v>
       </c>
-      <c r="D35" t="s">
-        <v>47</v>
+      <c r="D35" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E35" t="s">
         <v>44</v>
@@ -3665,76 +3326,78 @@
       <c r="F35" t="s">
         <v>36</v>
       </c>
-      <c r="G35" s="44"/>
+      <c r="G35" s="42" t="s">
+        <v>102</v>
+      </c>
       <c r="H35" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I35" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K35" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>ios</v>
       </c>
       <c r="L35" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M35" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>phone</v>
       </c>
       <c r="N35" s="6" t="s">
         <v>11</v>
       </c>
       <c r="O35" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>web</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>15</v>
       </c>
       <c r="Q35" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>safari</v>
       </c>
       <c r="R35" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S35" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T35" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U35" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V35" s="15" t="s">
         <v>4</v>
       </c>
       <c r="W35" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ios</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
         <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="D36" s="42" t="s">
+        <v>105</v>
       </c>
       <c r="E36" t="s">
         <v>28</v>
@@ -3742,76 +3405,78 @@
       <c r="F36" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="44"/>
+      <c r="G36" s="42" t="s">
+        <v>103</v>
+      </c>
       <c r="H36" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I36" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J36" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K36" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>ios</v>
       </c>
       <c r="L36" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M36" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>phone</v>
       </c>
       <c r="N36" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O36" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q36" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R36" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S36" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T36" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U36" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V36" s="15" t="s">
         <v>4</v>
       </c>
       <c r="W36" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ios</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
         <v>26</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>105</v>
       </c>
       <c r="E37" t="s">
         <v>29</v>
@@ -3819,67 +3484,69 @@
       <c r="F37" t="s">
         <v>36</v>
       </c>
-      <c r="G37" s="44"/>
+      <c r="G37" s="42" t="s">
+        <v>103</v>
+      </c>
       <c r="H37" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I37" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K37" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>ios</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M37" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>phone</v>
       </c>
       <c r="N37" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O37" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P37" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q37" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R37" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S37" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T37" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U37" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V37" s="15" t="s">
         <v>4</v>
       </c>
       <c r="W37" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ios</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
@@ -3887,8 +3554,8 @@
       <c r="C38" t="s">
         <v>34</v>
       </c>
-      <c r="D38" t="s">
-        <v>47</v>
+      <c r="D38" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="E38" t="s">
         <v>44</v>
@@ -3896,76 +3563,78 @@
       <c r="F38" t="s">
         <v>36</v>
       </c>
-      <c r="G38" s="44"/>
+      <c r="G38" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="H38" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I38" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J38" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K38" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>ios</v>
       </c>
       <c r="L38" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M38" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>tablet</v>
       </c>
       <c r="N38" s="6" t="s">
         <v>11</v>
       </c>
       <c r="O38" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>web</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>15</v>
       </c>
       <c r="Q38" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>safari</v>
       </c>
       <c r="R38" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S38" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T38" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U38" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V38" s="15" t="s">
         <v>4</v>
       </c>
       <c r="W38" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ios</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="D39" s="42" t="s">
+        <v>105</v>
       </c>
       <c r="E39" t="s">
         <v>28</v>
@@ -3973,76 +3642,78 @@
       <c r="F39" t="s">
         <v>36</v>
       </c>
-      <c r="G39" s="44"/>
+      <c r="G39" s="42" t="s">
+        <v>104</v>
+      </c>
       <c r="H39" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I39" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J39" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K39" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>ios</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M39" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>tablet</v>
       </c>
       <c r="N39" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O39" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P39" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q39" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R39" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S39" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T39" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U39" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V39" s="15" t="s">
         <v>4</v>
       </c>
       <c r="W39" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>ios</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>105</v>
       </c>
       <c r="E40" t="s">
         <v>29</v>
@@ -4050,528 +3721,542 @@
       <c r="F40" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="44"/>
+      <c r="G40" s="42" t="s">
+        <v>104</v>
+      </c>
       <c r="H40" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I40" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>touch</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>4</v>
       </c>
       <c r="K40" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>ios</v>
       </c>
       <c r="L40" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M40" s="14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>tablet</v>
       </c>
       <c r="N40" s="6" t="s">
         <v>10</v>
       </c>
       <c r="O40" s="14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>native</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q40" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="R40" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S40" s="14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>!hardware</v>
       </c>
       <c r="T40" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U40" s="14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>undefined</v>
       </c>
       <c r="V40" s="15" t="s">
         <v>4</v>
       </c>
       <c r="W40" s="14" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+        <v>ios</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E41" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="H41" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>N/A</v>
+      </c>
+      <c r="J41" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" s="47" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="L41" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="M41" s="47" t="str">
+        <f t="shared" si="2"/>
+        <v>N/A</v>
+      </c>
+      <c r="N41" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="O41" s="47" t="str">
+        <f t="shared" si="3"/>
+        <v>N/A</v>
+      </c>
+      <c r="P41" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q41" s="47" t="str">
+        <f t="shared" si="4"/>
+        <v>N/A</v>
+      </c>
+      <c r="R41" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="S41" s="47" t="str">
+        <f t="shared" si="5"/>
+        <v>N/A</v>
+      </c>
+      <c r="T41" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="U41" s="47" t="str">
+        <f t="shared" si="6"/>
+        <v>N/A</v>
+      </c>
+      <c r="V41" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="W41" s="47" t="str">
+        <f t="shared" si="7"/>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D42" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E42" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="H42" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>N/A</v>
+      </c>
+      <c r="J42" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="K42" s="47" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="L42" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" s="47" t="str">
+        <f t="shared" si="2"/>
+        <v>N/A</v>
+      </c>
+      <c r="N42" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="O42" s="47" t="str">
+        <f t="shared" si="3"/>
+        <v>N/A</v>
+      </c>
+      <c r="P42" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q42" s="47" t="str">
+        <f t="shared" si="4"/>
+        <v>N/A</v>
+      </c>
+      <c r="R42" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="S42" s="47" t="str">
+        <f t="shared" si="5"/>
+        <v>N/A</v>
+      </c>
+      <c r="T42" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="U42" s="47" t="str">
+        <f t="shared" si="6"/>
+        <v>N/A</v>
+      </c>
+      <c r="V42" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="W42" s="47" t="str">
+        <f t="shared" si="7"/>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E43" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="H43" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="I43" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>N/A</v>
+      </c>
+      <c r="J43" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="K43" s="47" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="L43" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="M43" s="47" t="str">
+        <f t="shared" si="2"/>
+        <v>N/A</v>
+      </c>
+      <c r="N43" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="O43" s="47" t="str">
+        <f t="shared" si="3"/>
+        <v>N/A</v>
+      </c>
+      <c r="P43" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q43" s="47" t="str">
+        <f t="shared" si="4"/>
+        <v>N/A</v>
+      </c>
+      <c r="R43" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="S43" s="47" t="str">
+        <f t="shared" si="5"/>
+        <v>N/A</v>
+      </c>
+      <c r="T43" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="U43" s="47" t="str">
+        <f t="shared" si="6"/>
+        <v>N/A</v>
+      </c>
+      <c r="V43" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="W43" s="47" t="str">
+        <f t="shared" si="7"/>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D44" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E44" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="H44" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="I44" s="47" t="str">
+        <f t="shared" si="0"/>
+        <v>N/A</v>
+      </c>
+      <c r="J44" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="K44" s="47" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="L44" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="M44" s="47" t="str">
+        <f t="shared" si="2"/>
+        <v>N/A</v>
+      </c>
+      <c r="N44" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="O44" s="47" t="str">
+        <f t="shared" si="3"/>
+        <v>N/A</v>
+      </c>
+      <c r="P44" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q44" s="47" t="str">
+        <f t="shared" si="4"/>
+        <v>N/A</v>
+      </c>
+      <c r="R44" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="S44" s="47" t="str">
+        <f t="shared" si="5"/>
+        <v>N/A</v>
+      </c>
+      <c r="T44" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="U44" s="47" t="str">
+        <f t="shared" si="6"/>
+        <v>N/A</v>
+      </c>
+      <c r="V44" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="W44" s="47" t="str">
+        <f t="shared" si="7"/>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="E41" t="s">
-        <v>44</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="B45" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E45" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G41" s="44"/>
-      <c r="H41" s="6" t="s">
+      <c r="G45" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="H45" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="I41" s="14" t="str">
+      <c r="I45" s="47" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J41" s="6" t="s">
+        <v>N/A</v>
+      </c>
+      <c r="J45" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K41" s="14" t="str">
+      <c r="K45" s="47" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M41" s="14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="L45" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="M45" s="47" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N41" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O41" s="14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="N45" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="O45" s="47" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="P41" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q41" s="14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P45" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q45" s="47" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="R41" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="S41" s="14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="R45" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="S45" s="47" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T41" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="U41" s="14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="T45" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="U45" s="47" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="V41" s="15" t="s">
+        <v>N/A</v>
+      </c>
+      <c r="V45" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="W41" s="14" t="str">
+      <c r="W45" s="47" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B42" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" t="s">
-        <v>28</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="D46" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E46" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G42" s="44"/>
-      <c r="H42" s="6" t="s">
+      <c r="G46" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="H46" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="I42" s="14" t="str">
+      <c r="I46" s="47" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J42" s="6" t="s">
+        <v>N/A</v>
+      </c>
+      <c r="J46" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="14" t="str">
+      <c r="K46" s="47" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M42" s="14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="L46" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="M46" s="47" t="str">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N42" s="6" t="s">
+        <v>N/A</v>
+      </c>
+      <c r="N46" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="O42" s="14" t="str">
+      <c r="O46" s="47" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="P42" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q42" s="14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="P46" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q46" s="47" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="R42" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="S42" s="14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="R46" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="S46" s="47" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T42" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="U42" s="14" t="str">
+        <v>N/A</v>
+      </c>
+      <c r="T46" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="U46" s="47" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="V42" s="15" t="s">
+        <v>N/A</v>
+      </c>
+      <c r="V46" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="W42" s="14" t="str">
+      <c r="W46" s="47" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" t="s">
-        <v>53</v>
-      </c>
-      <c r="E43" t="s">
-        <v>29</v>
-      </c>
-      <c r="F43" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" s="44"/>
-      <c r="H43" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I43" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K43" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M43" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N43" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O43" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="P43" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q43" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="R43" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="S43" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T43" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="U43" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="V43" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="W43" s="14" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" t="s">
-        <v>47</v>
-      </c>
-      <c r="E44" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44" s="44"/>
-      <c r="H44" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I44" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J44" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K44" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L44" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M44" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N44" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O44" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="P44" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q44" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="R44" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="S44" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T44" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="U44" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="V44" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="W44" s="14" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" t="s">
-        <v>28</v>
-      </c>
-      <c r="F45" t="s">
-        <v>27</v>
-      </c>
-      <c r="G45" s="44"/>
-      <c r="H45" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I45" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J45" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K45" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L45" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M45" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N45" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O45" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="P45" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q45" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="R45" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="S45" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T45" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="U45" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="V45" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="W45" s="14" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" t="s">
-        <v>49</v>
-      </c>
-      <c r="D46" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" t="s">
-        <v>29</v>
-      </c>
-      <c r="F46" t="s">
-        <v>27</v>
-      </c>
-      <c r="G46" s="44"/>
-      <c r="H46" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I46" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K46" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L46" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M46" s="14" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="N46" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O46" s="14" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="P46" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q46" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="R46" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="S46" s="14" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T46" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="U46" s="14" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="V46" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="W46" s="14" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <v>N/A</v>
       </c>
     </row>
     <row r="47" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G47" s="43"/>
+      <c r="G47" s="41"/>
       <c r="H47" s="21"/>
       <c r="I47" s="14" t="str">
         <f t="shared" si="0"/>
@@ -4617,7 +4302,7 @@
       <c r="A48" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G48" s="43"/>
+      <c r="G48" s="41"/>
       <c r="H48" s="21"/>
       <c r="I48" s="14" t="str">
         <f t="shared" si="0"/>
@@ -4669,14 +4354,17 @@
       <c r="C49" t="s">
         <v>34</v>
       </c>
+      <c r="D49" s="42" t="s">
+        <v>105</v>
+      </c>
       <c r="E49" t="s">
         <v>38</v>
       </c>
       <c r="F49" t="s">
         <v>36</v>
       </c>
-      <c r="G49" s="44" t="s">
-        <v>99</v>
+      <c r="G49" s="42" t="s">
+        <v>96</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>0</v>
@@ -4714,14 +4402,14 @@
         <v>chrome</v>
       </c>
       <c r="R49" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S49" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!hardware</v>
       </c>
       <c r="T49" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U49" s="14" t="str">
         <f t="shared" si="6"/>
@@ -4745,14 +4433,17 @@
       <c r="C50" t="s">
         <v>34</v>
       </c>
+      <c r="D50" s="42" t="s">
+        <v>105</v>
+      </c>
       <c r="E50" t="s">
         <v>38</v>
       </c>
       <c r="F50" t="s">
         <v>27</v>
       </c>
-      <c r="G50" s="44" t="s">
-        <v>98</v>
+      <c r="G50" s="42" t="s">
+        <v>95</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>1</v>
@@ -4790,14 +4481,14 @@
         <v>chrome</v>
       </c>
       <c r="R50" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S50" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T50" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U50" s="14" t="str">
         <f t="shared" si="6"/>
@@ -4821,14 +4512,17 @@
       <c r="C51" t="s">
         <v>34</v>
       </c>
+      <c r="D51" s="42" t="s">
+        <v>105</v>
+      </c>
       <c r="E51" t="s">
         <v>38</v>
       </c>
       <c r="F51" t="s">
         <v>36</v>
       </c>
-      <c r="G51" s="44" t="s">
-        <v>99</v>
+      <c r="G51" s="42" t="s">
+        <v>96</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>0</v>
@@ -4866,14 +4560,14 @@
         <v>chrome</v>
       </c>
       <c r="R51" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S51" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!hardware</v>
       </c>
       <c r="T51" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U51" s="14" t="str">
         <f t="shared" si="6"/>
@@ -4897,14 +4591,17 @@
       <c r="C52" t="s">
         <v>34</v>
       </c>
+      <c r="D52" s="42" t="s">
+        <v>105</v>
+      </c>
       <c r="E52" t="s">
         <v>38</v>
       </c>
       <c r="F52" t="s">
         <v>27</v>
       </c>
-      <c r="G52" s="44" t="s">
-        <v>98</v>
+      <c r="G52" s="42" t="s">
+        <v>95</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>1</v>
@@ -4942,14 +4639,14 @@
         <v>chrome</v>
       </c>
       <c r="R52" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S52" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T52" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U52" s="14" t="str">
         <f t="shared" si="6"/>
@@ -4973,14 +4670,17 @@
       <c r="C53" t="s">
         <v>34</v>
       </c>
+      <c r="D53" s="42" t="s">
+        <v>105</v>
+      </c>
       <c r="E53" t="s">
         <v>38</v>
       </c>
       <c r="F53" t="s">
         <v>36</v>
       </c>
-      <c r="G53" s="44" t="s">
-        <v>100</v>
+      <c r="G53" s="42" t="s">
+        <v>97</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>0</v>
@@ -5018,14 +4718,14 @@
         <v>safari</v>
       </c>
       <c r="R53" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S53" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!hardware</v>
       </c>
       <c r="T53" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U53" s="14" t="str">
         <f t="shared" si="6"/>
@@ -5049,14 +4749,17 @@
       <c r="C54" t="s">
         <v>34</v>
       </c>
+      <c r="D54" s="42" t="s">
+        <v>105</v>
+      </c>
       <c r="E54" t="s">
         <v>38</v>
       </c>
       <c r="F54" t="s">
         <v>27</v>
       </c>
-      <c r="G54" s="44" t="s">
-        <v>101</v>
+      <c r="G54" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>1</v>
@@ -5094,14 +4797,14 @@
         <v>safari</v>
       </c>
       <c r="R54" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S54" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T54" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U54" s="14" t="str">
         <f t="shared" si="6"/>
@@ -5125,14 +4828,17 @@
       <c r="C55" t="s">
         <v>34</v>
       </c>
+      <c r="D55" s="42" t="s">
+        <v>105</v>
+      </c>
       <c r="E55" t="s">
         <v>38</v>
       </c>
       <c r="F55" t="s">
         <v>36</v>
       </c>
-      <c r="G55" s="44" t="s">
-        <v>100</v>
+      <c r="G55" s="42" t="s">
+        <v>97</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>0</v>
@@ -5170,14 +4876,14 @@
         <v>safari</v>
       </c>
       <c r="R55" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S55" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!hardware</v>
       </c>
       <c r="T55" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U55" s="14" t="str">
         <f t="shared" si="6"/>
@@ -5201,14 +4907,17 @@
       <c r="C56" t="s">
         <v>34</v>
       </c>
+      <c r="D56" s="42" t="s">
+        <v>105</v>
+      </c>
       <c r="E56" t="s">
         <v>38</v>
       </c>
       <c r="F56" t="s">
         <v>27</v>
       </c>
-      <c r="G56" s="44" t="s">
-        <v>101</v>
+      <c r="G56" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>1</v>
@@ -5246,14 +4955,14 @@
         <v>safari</v>
       </c>
       <c r="R56" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S56" s="14" t="str">
         <f t="shared" si="5"/>
         <v>!touch</v>
       </c>
       <c r="T56" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U56" s="14" t="str">
         <f t="shared" si="6"/>
@@ -5268,7 +4977,7 @@
       </c>
     </row>
     <row r="57" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G57" s="43"/>
+      <c r="G57" s="41"/>
       <c r="H57" s="21"/>
       <c r="I57" s="20"/>
       <c r="J57" s="21"/>
@@ -5284,11 +4993,11 @@
       <c r="T57" s="19"/>
       <c r="U57" s="20"/>
       <c r="V57" s="23"/>
-      <c r="W57" s="28"/>
+      <c r="W57" s="26"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
@@ -5298,11 +5007,11 @@
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G61" s="43"/>
+      <c r="G61" s="41"/>
       <c r="H61" s="21"/>
       <c r="I61" s="20"/>
       <c r="J61" s="21"/>
@@ -5318,10 +5027,10 @@
       <c r="T61" s="19"/>
       <c r="U61" s="20"/>
       <c r="V61" s="23"/>
-      <c r="W61" s="28"/>
+      <c r="W61" s="26"/>
     </row>
     <row r="62" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G62" s="43"/>
+      <c r="G62" s="41"/>
       <c r="H62" s="21"/>
       <c r="I62" s="20"/>
       <c r="J62" s="21"/>
@@ -5337,10 +5046,10 @@
       <c r="T62" s="19"/>
       <c r="U62" s="20"/>
       <c r="V62" s="23"/>
-      <c r="W62" s="28"/>
+      <c r="W62" s="26"/>
     </row>
     <row r="63" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G63" s="43"/>
+      <c r="G63" s="41"/>
       <c r="H63" s="21"/>
       <c r="I63" s="20"/>
       <c r="J63" s="21"/>
@@ -5356,10 +5065,10 @@
       <c r="T63" s="19"/>
       <c r="U63" s="20"/>
       <c r="V63" s="23"/>
-      <c r="W63" s="28"/>
+      <c r="W63" s="26"/>
     </row>
     <row r="64" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G64" s="43"/>
+      <c r="G64" s="41"/>
       <c r="H64" s="21"/>
       <c r="I64" s="20"/>
       <c r="J64" s="21"/>
@@ -5375,10 +5084,10 @@
       <c r="T64" s="19"/>
       <c r="U64" s="20"/>
       <c r="V64" s="23"/>
-      <c r="W64" s="28"/>
+      <c r="W64" s="26"/>
     </row>
     <row r="65" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G65" s="43"/>
+      <c r="G65" s="41"/>
       <c r="H65" s="21"/>
       <c r="I65" s="20"/>
       <c r="J65" s="21"/>
@@ -5394,10 +5103,10 @@
       <c r="T65" s="19"/>
       <c r="U65" s="20"/>
       <c r="V65" s="23"/>
-      <c r="W65" s="28"/>
+      <c r="W65" s="26"/>
     </row>
     <row r="66" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G66" s="43"/>
+      <c r="G66" s="41"/>
       <c r="H66" s="21"/>
       <c r="I66" s="20"/>
       <c r="J66" s="21"/>
@@ -5413,10 +5122,10 @@
       <c r="T66" s="19"/>
       <c r="U66" s="20"/>
       <c r="V66" s="23"/>
-      <c r="W66" s="28"/>
+      <c r="W66" s="26"/>
     </row>
     <row r="67" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G67" s="43"/>
+      <c r="G67" s="41"/>
       <c r="H67" s="21"/>
       <c r="I67" s="20"/>
       <c r="J67" s="21"/>
@@ -5432,10 +5141,10 @@
       <c r="T67" s="19"/>
       <c r="U67" s="20"/>
       <c r="V67" s="23"/>
-      <c r="W67" s="28"/>
+      <c r="W67" s="26"/>
     </row>
     <row r="68" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G68" s="43"/>
+      <c r="G68" s="41"/>
       <c r="H68" s="21"/>
       <c r="I68" s="20"/>
       <c r="J68" s="21"/>
@@ -5451,10 +5160,10 @@
       <c r="T68" s="19"/>
       <c r="U68" s="20"/>
       <c r="V68" s="23"/>
-      <c r="W68" s="28"/>
+      <c r="W68" s="26"/>
     </row>
     <row r="69" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G69" s="43"/>
+      <c r="G69" s="41"/>
       <c r="H69" s="21"/>
       <c r="I69" s="20"/>
       <c r="J69" s="21"/>
@@ -5470,10 +5179,10 @@
       <c r="T69" s="19"/>
       <c r="U69" s="20"/>
       <c r="V69" s="23"/>
-      <c r="W69" s="28"/>
+      <c r="W69" s="26"/>
     </row>
     <row r="70" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G70" s="43"/>
+      <c r="G70" s="41"/>
       <c r="H70" s="21"/>
       <c r="I70" s="20"/>
       <c r="J70" s="21"/>
@@ -5489,10 +5198,10 @@
       <c r="T70" s="19"/>
       <c r="U70" s="20"/>
       <c r="V70" s="23"/>
-      <c r="W70" s="28"/>
+      <c r="W70" s="26"/>
     </row>
     <row r="71" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G71" s="43"/>
+      <c r="G71" s="41"/>
       <c r="H71" s="21"/>
       <c r="I71" s="20"/>
       <c r="J71" s="21"/>
@@ -5508,10 +5217,10 @@
       <c r="T71" s="19"/>
       <c r="U71" s="20"/>
       <c r="V71" s="23"/>
-      <c r="W71" s="28"/>
+      <c r="W71" s="26"/>
     </row>
     <row r="72" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G72" s="43"/>
+      <c r="G72" s="41"/>
       <c r="H72" s="21"/>
       <c r="I72" s="20"/>
       <c r="J72" s="21"/>
@@ -5527,10 +5236,10 @@
       <c r="T72" s="19"/>
       <c r="U72" s="20"/>
       <c r="V72" s="23"/>
-      <c r="W72" s="28"/>
+      <c r="W72" s="26"/>
     </row>
     <row r="73" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G73" s="43"/>
+      <c r="G73" s="41"/>
       <c r="H73" s="21"/>
       <c r="I73" s="20"/>
       <c r="J73" s="21"/>
@@ -5546,10 +5255,10 @@
       <c r="T73" s="19"/>
       <c r="U73" s="20"/>
       <c r="V73" s="23"/>
-      <c r="W73" s="28"/>
+      <c r="W73" s="26"/>
     </row>
     <row r="74" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G74" s="43"/>
+      <c r="G74" s="41"/>
       <c r="H74" s="21"/>
       <c r="I74" s="20"/>
       <c r="J74" s="21"/>
@@ -5565,10 +5274,10 @@
       <c r="T74" s="19"/>
       <c r="U74" s="20"/>
       <c r="V74" s="23"/>
-      <c r="W74" s="28"/>
+      <c r="W74" s="26"/>
     </row>
     <row r="75" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G75" s="43"/>
+      <c r="G75" s="41"/>
       <c r="H75" s="21"/>
       <c r="I75" s="20"/>
       <c r="J75" s="21"/>
@@ -5584,10 +5293,10 @@
       <c r="T75" s="19"/>
       <c r="U75" s="20"/>
       <c r="V75" s="23"/>
-      <c r="W75" s="28"/>
+      <c r="W75" s="26"/>
     </row>
     <row r="76" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G76" s="43"/>
+      <c r="G76" s="41"/>
       <c r="H76" s="21"/>
       <c r="I76" s="20"/>
       <c r="J76" s="21"/>
@@ -5603,10 +5312,10 @@
       <c r="T76" s="19"/>
       <c r="U76" s="20"/>
       <c r="V76" s="23"/>
-      <c r="W76" s="28"/>
+      <c r="W76" s="26"/>
     </row>
     <row r="77" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G77" s="43"/>
+      <c r="G77" s="41"/>
       <c r="H77" s="21"/>
       <c r="I77" s="20"/>
       <c r="J77" s="21"/>
@@ -5622,10 +5331,10 @@
       <c r="T77" s="19"/>
       <c r="U77" s="20"/>
       <c r="V77" s="23"/>
-      <c r="W77" s="28"/>
+      <c r="W77" s="26"/>
     </row>
     <row r="78" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G78" s="43"/>
+      <c r="G78" s="41"/>
       <c r="H78" s="21"/>
       <c r="I78" s="20"/>
       <c r="J78" s="21"/>
@@ -5641,10 +5350,10 @@
       <c r="T78" s="19"/>
       <c r="U78" s="20"/>
       <c r="V78" s="23"/>
-      <c r="W78" s="28"/>
+      <c r="W78" s="26"/>
     </row>
     <row r="79" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="G79" s="43"/>
+      <c r="G79" s="41"/>
       <c r="H79" s="21"/>
       <c r="I79" s="20"/>
       <c r="J79" s="21"/>
@@ -5660,16 +5369,10 @@
       <c r="T79" s="19"/>
       <c r="U79" s="20"/>
       <c r="V79" s="23"/>
-      <c r="W79" s="28"/>
+      <c r="W79" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P2:Q2"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="R1:S1"/>
@@ -5680,19 +5383,28 @@
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="T2:U2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P2:Q2"/>
   </mergeCells>
   <conditionalFormatting sqref="I6:I56 K6:K56 M6:M56 O6:O56 Q6:Q56 S6:S56 U6:U56 W6:W56">
-    <cfRule type="expression" priority="3" stopIfTrue="1">
+    <cfRule type="expression" priority="1" stopIfTrue="1">
       <formula>OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),0,-1)=""</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="26" priority="6" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(I6))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="7" stopIfTrue="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="8" stopIfTrue="1" operator="notEqual">
       <formula>OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),0,-1)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>OFFSET(INDIRECT(ADDRESS(ROW(), COLUMN())),0,-1)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"N/A"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Mac] Fixed logic to handle inverted (NOT_EQUAL) platform check
</commit_message>
<xml_diff>
--- a/windows/src/test/manual-tests/platform-rules/platform-results.xlsx
+++ b/windows/src/test/manual-tests/platform-rules/platform-results.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\keyman\open\windows\src\test\manual-tests\platform-rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/keymanapp/keyman/windows/src/test/manual-tests/platform-rules/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{443F142C-3122-544A-AA40-B86E9463E0A2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12240"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25120" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="116">
   <si>
     <t>touch</t>
   </si>
@@ -281,9 +282,6 @@
     <t>Token #</t>
   </si>
   <si>
-    <t>hardware macosx desktop native undefined undefined platform-x windows</t>
-  </si>
-  <si>
     <t>hardware windows desktop web chrome !touch undefined windows</t>
   </si>
   <si>
@@ -372,12 +370,15 @@
   </si>
   <si>
     <t>*not responding to hardware keyboard; separate issue?</t>
+  </si>
+  <si>
+    <t>hardware macosx desktop native undefined !touch undefined macosx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -592,12 +593,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -607,6 +602,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -960,114 +961,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X23" sqref="X23"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.1640625" style="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" style="6" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" style="14" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" style="22" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" style="14" customWidth="1"/>
-    <col min="22" max="22" width="9.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="10.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.6640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" style="22" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" style="14" customWidth="1"/>
+    <col min="22" max="22" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="9" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G1" s="38"/>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="43" t="s">
+      <c r="I1" s="48"/>
+      <c r="J1" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="44"/>
-      <c r="L1" s="43" t="s">
+      <c r="K1" s="48"/>
+      <c r="L1" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="44"/>
-      <c r="N1" s="43" t="s">
+      <c r="M1" s="48"/>
+      <c r="N1" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="44"/>
-      <c r="P1" s="43" t="s">
+      <c r="O1" s="48"/>
+      <c r="P1" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="43" t="s">
+      <c r="Q1" s="48"/>
+      <c r="R1" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="S1" s="44"/>
-      <c r="T1" s="43" t="s">
+      <c r="S1" s="48"/>
+      <c r="T1" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="U1" s="44"/>
-      <c r="V1" s="43" t="s">
+      <c r="U1" s="48"/>
+      <c r="V1" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="44"/>
-    </row>
-    <row r="2" spans="1:23" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="W1" s="48"/>
+    </row>
+    <row r="2" spans="1:23" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="G2" s="38"/>
-      <c r="H2" s="43" t="s">
+      <c r="H2" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="43" t="s">
+      <c r="I2" s="48"/>
+      <c r="J2" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="43" t="s">
+      <c r="K2" s="48"/>
+      <c r="L2" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="M2" s="44"/>
-      <c r="N2" s="43" t="s">
+      <c r="M2" s="48"/>
+      <c r="N2" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="43" t="s">
+      <c r="O2" s="48"/>
+      <c r="P2" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="Q2" s="48"/>
+      <c r="R2" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="S2" s="44"/>
-      <c r="T2" s="43" t="s">
+      <c r="S2" s="48"/>
+      <c r="T2" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="U2" s="44"/>
-      <c r="V2" s="43" t="s">
+      <c r="U2" s="48"/>
+      <c r="V2" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="W2" s="44"/>
-    </row>
-    <row r="3" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W2" s="48"/>
+    </row>
+    <row r="3" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
@@ -1138,7 +1139,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="31" customFormat="1" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="31" customFormat="1" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
         <v>84</v>
       </c>
@@ -1176,7 +1177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G5" s="40"/>
       <c r="H5" s="28"/>
       <c r="I5" s="27"/>
@@ -1195,7 +1196,7 @@
       <c r="V5" s="23"/>
       <c r="W5" s="26"/>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>windows</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1348,7 +1349,7 @@
         <v>windows</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1356,7 +1357,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
         <v>21</v>
@@ -1365,7 +1366,7 @@
         <v>27</v>
       </c>
       <c r="G8" s="42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>1</v>
@@ -1424,7 +1425,7 @@
         <v>windows</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>34</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
         <v>45</v>
@@ -1441,7 +1442,7 @@
         <v>27</v>
       </c>
       <c r="G9" s="42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H9" s="18" t="s">
         <v>1</v>
@@ -1500,7 +1501,7 @@
         <v>windows</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>34</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
@@ -1517,7 +1518,7 @@
         <v>27</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H10" s="18" t="s">
         <v>1</v>
@@ -1576,7 +1577,7 @@
         <v>windows</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1584,7 +1585,7 @@
         <v>34</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
         <v>42</v>
@@ -1593,7 +1594,7 @@
         <v>27</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H11" s="18" t="s">
         <v>1</v>
@@ -1652,7 +1653,7 @@
         <v>windows</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1660,7 +1661,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" t="s">
         <v>41</v>
@@ -1669,7 +1670,7 @@
         <v>27</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H12" s="18" t="s">
         <v>1</v>
@@ -1728,7 +1729,7 @@
         <v>windows</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G13" s="41"/>
       <c r="H13" s="21"/>
       <c r="I13" s="14" t="str">
@@ -1771,7 +1772,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1788,7 +1789,7 @@
         <v>27</v>
       </c>
       <c r="G14" s="42" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>1</v>
@@ -1830,24 +1831,24 @@
       </c>
       <c r="S14" s="14" t="str">
         <f t="shared" si="5"/>
-        <v>undefined</v>
+        <v>!touch</v>
       </c>
       <c r="T14" s="16" t="s">
         <v>49</v>
       </c>
       <c r="U14" s="14" t="str">
         <f t="shared" si="6"/>
-        <v>platform-x</v>
+        <v>undefined</v>
       </c>
       <c r="V14" s="15" t="s">
         <v>5</v>
       </c>
       <c r="W14" s="14" t="str">
         <f t="shared" si="7"/>
-        <v>windows</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+        <v>macosx</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E15" t="s">
         <v>21</v>
@@ -1864,7 +1865,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>1</v>
@@ -1923,7 +1924,7 @@
         <v>macosx</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1931,7 +1932,7 @@
         <v>34</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
         <v>44</v>
@@ -1940,7 +1941,7 @@
         <v>27</v>
       </c>
       <c r="G16" s="42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>1</v>
@@ -1999,7 +2000,7 @@
         <v>macosx</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -2007,7 +2008,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E17" t="s">
         <v>41</v>
@@ -2016,7 +2017,7 @@
         <v>27</v>
       </c>
       <c r="G17" s="42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>1</v>
@@ -2075,7 +2076,7 @@
         <v>macosx</v>
       </c>
     </row>
-    <row r="18" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G18" s="41"/>
       <c r="H18" s="21"/>
       <c r="I18" s="14" t="str">
@@ -2118,7 +2119,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2126,7 +2127,7 @@
         <v>34</v>
       </c>
       <c r="D19" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
@@ -2135,7 +2136,7 @@
         <v>27</v>
       </c>
       <c r="G19" s="42" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>1</v>
@@ -2194,7 +2195,7 @@
         <v>linux</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -2202,7 +2203,7 @@
         <v>34</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E20" t="s">
         <v>41</v>
@@ -2211,7 +2212,7 @@
         <v>27</v>
       </c>
       <c r="G20" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>1</v>
@@ -2270,7 +2271,7 @@
         <v>linux</v>
       </c>
     </row>
-    <row r="21" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G21" s="41"/>
       <c r="H21" s="21"/>
       <c r="I21" s="14" t="str">
@@ -2313,7 +2314,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -2324,7 +2325,7 @@
         <v>34</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E22" t="s">
         <v>21</v>
@@ -2333,7 +2334,7 @@
         <v>36</v>
       </c>
       <c r="G22" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>0</v>
@@ -2392,7 +2393,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2403,7 +2404,7 @@
         <v>34</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
         <v>21</v>
@@ -2412,7 +2413,7 @@
         <v>27</v>
       </c>
       <c r="G23" s="42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>1</v>
@@ -2471,10 +2472,10 @@
         <v>N/A</v>
       </c>
       <c r="X23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>35</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E24" t="s">
         <v>28</v>
@@ -2494,7 +2495,7 @@
         <v>36</v>
       </c>
       <c r="G24" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>0</v>
@@ -2553,7 +2554,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -2564,7 +2565,7 @@
         <v>35</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
@@ -2573,7 +2574,7 @@
         <v>27</v>
       </c>
       <c r="G25" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>1</v>
@@ -2632,7 +2633,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2643,7 +2644,7 @@
         <v>35</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E26" t="s">
         <v>29</v>
@@ -2652,7 +2653,7 @@
         <v>36</v>
       </c>
       <c r="G26" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>0</v>
@@ -2711,7 +2712,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2722,7 +2723,7 @@
         <v>35</v>
       </c>
       <c r="D27" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E27" t="s">
         <v>29</v>
@@ -2731,7 +2732,7 @@
         <v>27</v>
       </c>
       <c r="G27" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>1</v>
@@ -2790,7 +2791,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -2801,7 +2802,7 @@
         <v>34</v>
       </c>
       <c r="D28" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E28" t="s">
         <v>21</v>
@@ -2810,7 +2811,7 @@
         <v>36</v>
       </c>
       <c r="G28" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>0</v>
@@ -2869,7 +2870,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -2880,7 +2881,7 @@
         <v>34</v>
       </c>
       <c r="D29" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E29" t="s">
         <v>21</v>
@@ -2889,7 +2890,7 @@
         <v>27</v>
       </c>
       <c r="G29" s="42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>1</v>
@@ -2948,7 +2949,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -2959,7 +2960,7 @@
         <v>35</v>
       </c>
       <c r="D30" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E30" t="s">
         <v>28</v>
@@ -2968,7 +2969,7 @@
         <v>36</v>
       </c>
       <c r="G30" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H30" s="6" t="s">
         <v>0</v>
@@ -3027,7 +3028,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -3038,7 +3039,7 @@
         <v>35</v>
       </c>
       <c r="D31" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E31" t="s">
         <v>28</v>
@@ -3047,7 +3048,7 @@
         <v>27</v>
       </c>
       <c r="G31" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>1</v>
@@ -3106,7 +3107,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -3117,7 +3118,7 @@
         <v>35</v>
       </c>
       <c r="D32" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E32" t="s">
         <v>56</v>
@@ -3126,7 +3127,7 @@
         <v>36</v>
       </c>
       <c r="G32" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>0</v>
@@ -3185,7 +3186,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>57</v>
       </c>
@@ -3196,7 +3197,7 @@
         <v>35</v>
       </c>
       <c r="D33" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E33" t="s">
         <v>56</v>
@@ -3205,7 +3206,7 @@
         <v>27</v>
       </c>
       <c r="G33" s="42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>1</v>
@@ -3264,7 +3265,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G34" s="41"/>
       <c r="H34" s="21"/>
       <c r="I34" s="14" t="str">
@@ -3307,7 +3308,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -3318,7 +3319,7 @@
         <v>34</v>
       </c>
       <c r="D35" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E35" t="s">
         <v>44</v>
@@ -3327,7 +3328,7 @@
         <v>36</v>
       </c>
       <c r="G35" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>0</v>
@@ -3386,7 +3387,7 @@
         <v>ios</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -3397,7 +3398,7 @@
         <v>48</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E36" t="s">
         <v>28</v>
@@ -3406,7 +3407,7 @@
         <v>36</v>
       </c>
       <c r="G36" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H36" s="6" t="s">
         <v>0</v>
@@ -3465,7 +3466,7 @@
         <v>ios</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -3476,7 +3477,7 @@
         <v>48</v>
       </c>
       <c r="D37" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E37" t="s">
         <v>29</v>
@@ -3485,7 +3486,7 @@
         <v>36</v>
       </c>
       <c r="G37" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>0</v>
@@ -3544,7 +3545,7 @@
         <v>ios</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -3555,7 +3556,7 @@
         <v>34</v>
       </c>
       <c r="D38" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E38" t="s">
         <v>44</v>
@@ -3564,7 +3565,7 @@
         <v>36</v>
       </c>
       <c r="G38" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>0</v>
@@ -3623,7 +3624,7 @@
         <v>ios</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -3634,7 +3635,7 @@
         <v>48</v>
       </c>
       <c r="D39" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E39" t="s">
         <v>28</v>
@@ -3643,7 +3644,7 @@
         <v>36</v>
       </c>
       <c r="G39" s="42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>0</v>
@@ -3702,7 +3703,7 @@
         <v>ios</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>47</v>
       </c>
@@ -3713,7 +3714,7 @@
         <v>48</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40" t="s">
         <v>29</v>
@@ -3722,7 +3723,7 @@
         <v>36</v>
       </c>
       <c r="G40" s="42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>0</v>
@@ -3781,481 +3782,481 @@
         <v>ios</v>
       </c>
     </row>
-    <row r="41" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="45" t="s">
+    <row r="41" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="45" t="s">
+      <c r="B41" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="43" t="s">
         <v>34</v>
       </c>
       <c r="D41" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="45" t="s">
+      <c r="H41" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>N/A</v>
+      </c>
+      <c r="J41" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="L41" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="M41" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>N/A</v>
+      </c>
+      <c r="N41" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="O41" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>N/A</v>
+      </c>
+      <c r="P41" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q41" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>N/A</v>
+      </c>
+      <c r="R41" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="S41" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>N/A</v>
+      </c>
+      <c r="T41" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="U41" s="45" t="str">
+        <f t="shared" si="6"/>
+        <v>N/A</v>
+      </c>
+      <c r="V41" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="W41" s="45" t="str">
+        <f t="shared" si="7"/>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E42" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="H42" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>N/A</v>
+      </c>
+      <c r="J42" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K42" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="L42" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="M42" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>N/A</v>
+      </c>
+      <c r="N42" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="O42" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>N/A</v>
+      </c>
+      <c r="P42" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q42" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>N/A</v>
+      </c>
+      <c r="R42" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="S42" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>N/A</v>
+      </c>
+      <c r="T42" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="U42" s="45" t="str">
+        <f t="shared" si="6"/>
+        <v>N/A</v>
+      </c>
+      <c r="V42" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="W42" s="45" t="str">
+        <f t="shared" si="7"/>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="H43" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="I43" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>N/A</v>
+      </c>
+      <c r="J43" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K43" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="L43" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="M43" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>N/A</v>
+      </c>
+      <c r="N43" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="O43" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>N/A</v>
+      </c>
+      <c r="P43" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q43" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>N/A</v>
+      </c>
+      <c r="R43" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="S43" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>N/A</v>
+      </c>
+      <c r="T43" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="U43" s="45" t="str">
+        <f t="shared" si="6"/>
+        <v>N/A</v>
+      </c>
+      <c r="V43" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="W43" s="45" t="str">
+        <f t="shared" si="7"/>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="45" t="s">
+      <c r="F44" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="G41" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="H41" s="46" t="s">
+      <c r="G44" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="H44" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="I41" s="47" t="str">
+      <c r="I44" s="45" t="str">
         <f t="shared" si="0"/>
         <v>N/A</v>
       </c>
-      <c r="J41" s="46" t="s">
+      <c r="J44" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K41" s="47" t="str">
+      <c r="K44" s="45" t="str">
         <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
-      <c r="L41" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="M41" s="47" t="str">
+      <c r="L44" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M44" s="45" t="str">
         <f t="shared" si="2"/>
         <v>N/A</v>
       </c>
-      <c r="N41" s="46" t="s">
+      <c r="N44" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="O41" s="47" t="str">
+      <c r="O44" s="45" t="str">
         <f t="shared" si="3"/>
         <v>N/A</v>
       </c>
-      <c r="P41" s="46" t="s">
+      <c r="P44" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="Q41" s="47" t="str">
+      <c r="Q44" s="45" t="str">
         <f t="shared" si="4"/>
         <v>N/A</v>
       </c>
-      <c r="R41" s="46" t="s">
+      <c r="R44" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="S41" s="47" t="str">
+      <c r="S44" s="45" t="str">
         <f t="shared" si="5"/>
         <v>N/A</v>
       </c>
-      <c r="T41" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="U41" s="47" t="str">
+      <c r="T44" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="U44" s="45" t="str">
         <f t="shared" si="6"/>
         <v>N/A</v>
       </c>
-      <c r="V41" s="46" t="s">
+      <c r="V44" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="W41" s="47" t="str">
+      <c r="W44" s="45" t="str">
         <f t="shared" si="7"/>
         <v>N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
+    <row r="45" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="45" t="s">
+      <c r="B45" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="42" t="s">
+      <c r="D45" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="E42" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="F42" s="45" t="s">
+      <c r="H45" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="I45" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v>N/A</v>
+      </c>
+      <c r="J45" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K45" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v>N/A</v>
+      </c>
+      <c r="L45" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M45" s="45" t="str">
+        <f t="shared" si="2"/>
+        <v>N/A</v>
+      </c>
+      <c r="N45" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="O45" s="45" t="str">
+        <f t="shared" si="3"/>
+        <v>N/A</v>
+      </c>
+      <c r="P45" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q45" s="45" t="str">
+        <f t="shared" si="4"/>
+        <v>N/A</v>
+      </c>
+      <c r="R45" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="S45" s="45" t="str">
+        <f t="shared" si="5"/>
+        <v>N/A</v>
+      </c>
+      <c r="T45" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="U45" s="45" t="str">
+        <f t="shared" si="6"/>
+        <v>N/A</v>
+      </c>
+      <c r="V45" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="W45" s="45" t="str">
+        <f t="shared" si="7"/>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="G42" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="H42" s="46" t="s">
+      <c r="G46" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="H46" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="I42" s="47" t="str">
+      <c r="I46" s="45" t="str">
         <f t="shared" si="0"/>
         <v>N/A</v>
       </c>
-      <c r="J42" s="46" t="s">
+      <c r="J46" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="47" t="str">
+      <c r="K46" s="45" t="str">
         <f t="shared" si="1"/>
         <v>N/A</v>
       </c>
-      <c r="L42" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="M42" s="47" t="str">
+      <c r="L46" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="M46" s="45" t="str">
         <f t="shared" si="2"/>
         <v>N/A</v>
       </c>
-      <c r="N42" s="46" t="s">
+      <c r="N46" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="O42" s="47" t="str">
+      <c r="O46" s="45" t="str">
         <f t="shared" si="3"/>
         <v>N/A</v>
       </c>
-      <c r="P42" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q42" s="47" t="str">
+      <c r="P46" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q46" s="45" t="str">
         <f t="shared" si="4"/>
         <v>N/A</v>
       </c>
-      <c r="R42" s="46" t="s">
+      <c r="R46" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="S42" s="47" t="str">
+      <c r="S46" s="45" t="str">
         <f t="shared" si="5"/>
         <v>N/A</v>
       </c>
-      <c r="T42" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="U42" s="47" t="str">
+      <c r="T46" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="U46" s="45" t="str">
         <f t="shared" si="6"/>
         <v>N/A</v>
       </c>
-      <c r="V42" s="46" t="s">
+      <c r="V46" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="W42" s="47" t="str">
+      <c r="W46" s="45" t="str">
         <f t="shared" si="7"/>
         <v>N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="E43" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="F43" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="H43" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="I43" s="47" t="str">
-        <f t="shared" si="0"/>
-        <v>N/A</v>
-      </c>
-      <c r="J43" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="K43" s="47" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
-      <c r="L43" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="M43" s="47" t="str">
-        <f t="shared" si="2"/>
-        <v>N/A</v>
-      </c>
-      <c r="N43" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="O43" s="47" t="str">
-        <f t="shared" si="3"/>
-        <v>N/A</v>
-      </c>
-      <c r="P43" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q43" s="47" t="str">
-        <f t="shared" si="4"/>
-        <v>N/A</v>
-      </c>
-      <c r="R43" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="S43" s="47" t="str">
-        <f t="shared" si="5"/>
-        <v>N/A</v>
-      </c>
-      <c r="T43" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="U43" s="47" t="str">
-        <f t="shared" si="6"/>
-        <v>N/A</v>
-      </c>
-      <c r="V43" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="W43" s="47" t="str">
-        <f t="shared" si="7"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="E44" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="F44" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="H44" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="I44" s="47" t="str">
-        <f t="shared" si="0"/>
-        <v>N/A</v>
-      </c>
-      <c r="J44" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="K44" s="47" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
-      <c r="L44" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="M44" s="47" t="str">
-        <f t="shared" si="2"/>
-        <v>N/A</v>
-      </c>
-      <c r="N44" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="O44" s="47" t="str">
-        <f t="shared" si="3"/>
-        <v>N/A</v>
-      </c>
-      <c r="P44" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q44" s="47" t="str">
-        <f t="shared" si="4"/>
-        <v>N/A</v>
-      </c>
-      <c r="R44" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="S44" s="47" t="str">
-        <f t="shared" si="5"/>
-        <v>N/A</v>
-      </c>
-      <c r="T44" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="U44" s="47" t="str">
-        <f t="shared" si="6"/>
-        <v>N/A</v>
-      </c>
-      <c r="V44" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="W44" s="47" t="str">
-        <f t="shared" si="7"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C45" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="D45" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="E45" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="F45" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="G45" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="H45" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="I45" s="47" t="str">
-        <f t="shared" si="0"/>
-        <v>N/A</v>
-      </c>
-      <c r="J45" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="K45" s="47" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
-      <c r="L45" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="M45" s="47" t="str">
-        <f t="shared" si="2"/>
-        <v>N/A</v>
-      </c>
-      <c r="N45" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="O45" s="47" t="str">
-        <f t="shared" si="3"/>
-        <v>N/A</v>
-      </c>
-      <c r="P45" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q45" s="47" t="str">
-        <f t="shared" si="4"/>
-        <v>N/A</v>
-      </c>
-      <c r="R45" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="S45" s="47" t="str">
-        <f t="shared" si="5"/>
-        <v>N/A</v>
-      </c>
-      <c r="T45" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="U45" s="47" t="str">
-        <f t="shared" si="6"/>
-        <v>N/A</v>
-      </c>
-      <c r="V45" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="W45" s="47" t="str">
-        <f t="shared" si="7"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C46" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="E46" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="F46" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="G46" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="H46" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="I46" s="47" t="str">
-        <f t="shared" si="0"/>
-        <v>N/A</v>
-      </c>
-      <c r="J46" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="K46" s="47" t="str">
-        <f t="shared" si="1"/>
-        <v>N/A</v>
-      </c>
-      <c r="L46" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="M46" s="47" t="str">
-        <f t="shared" si="2"/>
-        <v>N/A</v>
-      </c>
-      <c r="N46" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="O46" s="47" t="str">
-        <f t="shared" si="3"/>
-        <v>N/A</v>
-      </c>
-      <c r="P46" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q46" s="47" t="str">
-        <f t="shared" si="4"/>
-        <v>N/A</v>
-      </c>
-      <c r="R46" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="S46" s="47" t="str">
-        <f t="shared" si="5"/>
-        <v>N/A</v>
-      </c>
-      <c r="T46" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="U46" s="47" t="str">
-        <f t="shared" si="6"/>
-        <v>N/A</v>
-      </c>
-      <c r="V46" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="W46" s="47" t="str">
-        <f t="shared" si="7"/>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G47" s="41"/>
       <c r="H47" s="21"/>
       <c r="I47" s="14" t="str">
@@ -4298,7 +4299,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="12" t="s">
         <v>38</v>
       </c>
@@ -4344,7 +4345,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>20</v>
       </c>
@@ -4355,7 +4356,7 @@
         <v>34</v>
       </c>
       <c r="D49" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E49" t="s">
         <v>38</v>
@@ -4364,7 +4365,7 @@
         <v>36</v>
       </c>
       <c r="G49" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H49" s="6" t="s">
         <v>0</v>
@@ -4423,7 +4424,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -4434,7 +4435,7 @@
         <v>34</v>
       </c>
       <c r="D50" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E50" t="s">
         <v>38</v>
@@ -4443,7 +4444,7 @@
         <v>27</v>
       </c>
       <c r="G50" s="42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>1</v>
@@ -4502,7 +4503,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -4513,7 +4514,7 @@
         <v>34</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E51" t="s">
         <v>38</v>
@@ -4522,7 +4523,7 @@
         <v>36</v>
       </c>
       <c r="G51" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>0</v>
@@ -4581,7 +4582,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>20</v>
       </c>
@@ -4592,7 +4593,7 @@
         <v>34</v>
       </c>
       <c r="D52" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E52" t="s">
         <v>38</v>
@@ -4601,7 +4602,7 @@
         <v>27</v>
       </c>
       <c r="G52" s="42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>1</v>
@@ -4660,7 +4661,7 @@
         <v>android</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>20</v>
       </c>
@@ -4671,7 +4672,7 @@
         <v>34</v>
       </c>
       <c r="D53" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E53" t="s">
         <v>38</v>
@@ -4680,7 +4681,7 @@
         <v>36</v>
       </c>
       <c r="G53" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>0</v>
@@ -4739,7 +4740,7 @@
         <v>ios</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -4750,7 +4751,7 @@
         <v>34</v>
       </c>
       <c r="D54" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E54" t="s">
         <v>38</v>
@@ -4759,7 +4760,7 @@
         <v>27</v>
       </c>
       <c r="G54" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>1</v>
@@ -4818,7 +4819,7 @@
         <v>ios</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -4829,7 +4830,7 @@
         <v>34</v>
       </c>
       <c r="D55" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E55" t="s">
         <v>38</v>
@@ -4838,7 +4839,7 @@
         <v>36</v>
       </c>
       <c r="G55" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>0</v>
@@ -4897,7 +4898,7 @@
         <v>ios</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -4908,7 +4909,7 @@
         <v>34</v>
       </c>
       <c r="D56" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E56" t="s">
         <v>38</v>
@@ -4917,7 +4918,7 @@
         <v>27</v>
       </c>
       <c r="G56" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>1</v>
@@ -4976,7 +4977,7 @@
         <v>ios</v>
       </c>
     </row>
-    <row r="57" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G57" s="41"/>
       <c r="H57" s="21"/>
       <c r="I57" s="20"/>
@@ -4995,22 +4996,22 @@
       <c r="V57" s="23"/>
       <c r="W57" s="26"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G61" s="41"/>
       <c r="H61" s="21"/>
       <c r="I61" s="20"/>
@@ -5029,7 +5030,7 @@
       <c r="V61" s="23"/>
       <c r="W61" s="26"/>
     </row>
-    <row r="62" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G62" s="41"/>
       <c r="H62" s="21"/>
       <c r="I62" s="20"/>
@@ -5048,7 +5049,7 @@
       <c r="V62" s="23"/>
       <c r="W62" s="26"/>
     </row>
-    <row r="63" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G63" s="41"/>
       <c r="H63" s="21"/>
       <c r="I63" s="20"/>
@@ -5067,7 +5068,7 @@
       <c r="V63" s="23"/>
       <c r="W63" s="26"/>
     </row>
-    <row r="64" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G64" s="41"/>
       <c r="H64" s="21"/>
       <c r="I64" s="20"/>
@@ -5086,7 +5087,7 @@
       <c r="V64" s="23"/>
       <c r="W64" s="26"/>
     </row>
-    <row r="65" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G65" s="41"/>
       <c r="H65" s="21"/>
       <c r="I65" s="20"/>
@@ -5105,7 +5106,7 @@
       <c r="V65" s="23"/>
       <c r="W65" s="26"/>
     </row>
-    <row r="66" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G66" s="41"/>
       <c r="H66" s="21"/>
       <c r="I66" s="20"/>
@@ -5124,7 +5125,7 @@
       <c r="V66" s="23"/>
       <c r="W66" s="26"/>
     </row>
-    <row r="67" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G67" s="41"/>
       <c r="H67" s="21"/>
       <c r="I67" s="20"/>
@@ -5143,7 +5144,7 @@
       <c r="V67" s="23"/>
       <c r="W67" s="26"/>
     </row>
-    <row r="68" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G68" s="41"/>
       <c r="H68" s="21"/>
       <c r="I68" s="20"/>
@@ -5162,7 +5163,7 @@
       <c r="V68" s="23"/>
       <c r="W68" s="26"/>
     </row>
-    <row r="69" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G69" s="41"/>
       <c r="H69" s="21"/>
       <c r="I69" s="20"/>
@@ -5181,7 +5182,7 @@
       <c r="V69" s="23"/>
       <c r="W69" s="26"/>
     </row>
-    <row r="70" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G70" s="41"/>
       <c r="H70" s="21"/>
       <c r="I70" s="20"/>
@@ -5200,7 +5201,7 @@
       <c r="V70" s="23"/>
       <c r="W70" s="26"/>
     </row>
-    <row r="71" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G71" s="41"/>
       <c r="H71" s="21"/>
       <c r="I71" s="20"/>
@@ -5219,7 +5220,7 @@
       <c r="V71" s="23"/>
       <c r="W71" s="26"/>
     </row>
-    <row r="72" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G72" s="41"/>
       <c r="H72" s="21"/>
       <c r="I72" s="20"/>
@@ -5238,7 +5239,7 @@
       <c r="V72" s="23"/>
       <c r="W72" s="26"/>
     </row>
-    <row r="73" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G73" s="41"/>
       <c r="H73" s="21"/>
       <c r="I73" s="20"/>
@@ -5257,7 +5258,7 @@
       <c r="V73" s="23"/>
       <c r="W73" s="26"/>
     </row>
-    <row r="74" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G74" s="41"/>
       <c r="H74" s="21"/>
       <c r="I74" s="20"/>
@@ -5276,7 +5277,7 @@
       <c r="V74" s="23"/>
       <c r="W74" s="26"/>
     </row>
-    <row r="75" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G75" s="41"/>
       <c r="H75" s="21"/>
       <c r="I75" s="20"/>
@@ -5295,7 +5296,7 @@
       <c r="V75" s="23"/>
       <c r="W75" s="26"/>
     </row>
-    <row r="76" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G76" s="41"/>
       <c r="H76" s="21"/>
       <c r="I76" s="20"/>
@@ -5314,7 +5315,7 @@
       <c r="V76" s="23"/>
       <c r="W76" s="26"/>
     </row>
-    <row r="77" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G77" s="41"/>
       <c r="H77" s="21"/>
       <c r="I77" s="20"/>
@@ -5333,7 +5334,7 @@
       <c r="V77" s="23"/>
       <c r="W77" s="26"/>
     </row>
-    <row r="78" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G78" s="41"/>
       <c r="H78" s="21"/>
       <c r="I78" s="20"/>
@@ -5352,7 +5353,7 @@
       <c r="V78" s="23"/>
       <c r="W78" s="26"/>
     </row>
-    <row r="79" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="G79" s="41"/>
       <c r="H79" s="21"/>
       <c r="I79" s="20"/>

</xml_diff>